<commit_message>
Excel Acabados Lectura de los excel y guardado de los datos
</commit_message>
<xml_diff>
--- a/DatosEstablecimiento.xlsx
+++ b/DatosEstablecimiento.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Desktop\AutoDatosViajeros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DatosViajeros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F6AF1E-D8A2-47A9-8C9F-E2F889D7162C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06E8BCB-2E42-4D04-AB02-BAB4EB22DDEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21690" yWindow="-1720" windowWidth="21780" windowHeight="18930" xr2:uid="{6EE986A1-B3DF-42F7-9F4A-D5934D58D2EE}"/>
+    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{6EE986A1-B3DF-42F7-9F4A-D5934D58D2EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <author>tc={7319482D-45D3-4598-9B6B-82C0B46E3760}</author>
   </authors>
   <commentList>
-    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{7319482D-45D3-4598-9B6B-82C0B46E3760}">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{7319482D-45D3-4598-9B6B-82C0B46E3760}">
       <text>
         <t xml:space="preserve">[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Código del establecimiento</t>
   </si>
@@ -84,13 +84,37 @@
   </si>
   <si>
     <t>Correo electrónico</t>
+  </si>
+  <si>
+    <t>falso1324</t>
+  </si>
+  <si>
+    <t>CASA_RURAL</t>
+  </si>
+  <si>
+    <t>calle falsa 123</t>
+  </si>
+  <si>
+    <t>Mentiras Rurales</t>
+  </si>
+  <si>
+    <t>Valencia</t>
+  </si>
+  <si>
+    <t>Aldaia</t>
+  </si>
+  <si>
+    <t>ESP</t>
+  </si>
+  <si>
+    <t>a@a.es</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +126,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -182,17 +214,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -531,7 +566,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="I3" dT="2025-03-23T21:20:56.30" personId="{C6D85F25-90A3-45AE-876B-34E5EE88D69D}" id="{7319482D-45D3-4598-9B6B-82C0B46E3760}">
+  <threadedComment ref="H2" dT="2025-03-23T21:20:56.30" personId="{C6D85F25-90A3-45AE-876B-34E5EE88D69D}" id="{7319482D-45D3-4598-9B6B-82C0B46E3760}">
     <text xml:space="preserve">BUSCAR código de país ISO 3166-1 </text>
   </threadedComment>
 </ThreadedComments>
@@ -539,72 +574,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25D2744-BE09-43A9-945D-78C1720AF83C}">
-  <dimension ref="B1:K63"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2">
+        <v>46111</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2">
+        <v>13245678</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -614,9 +681,9 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -626,9 +693,9 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -638,9 +705,9 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -650,9 +717,9 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -662,9 +729,9 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -674,9 +741,9 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -686,9 +753,9 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -698,9 +765,9 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -710,9 +777,9 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -722,9 +789,9 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -734,9 +801,9 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -746,9 +813,9 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -758,9 +825,9 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -770,9 +837,9 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -782,9 +849,9 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -794,9 +861,9 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -806,9 +873,9 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -818,9 +885,9 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -830,9 +897,9 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -842,9 +909,9 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -854,9 +921,9 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -866,9 +933,9 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -878,9 +945,9 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -890,9 +957,9 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -902,9 +969,9 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -914,9 +981,9 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -926,9 +993,9 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -938,9 +1005,9 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -950,9 +1017,9 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -962,9 +1029,9 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -974,9 +1041,9 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -986,9 +1053,9 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -998,9 +1065,9 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1010,9 +1077,9 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1022,9 +1089,9 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1034,9 +1101,9 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -1046,9 +1113,9 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -1058,9 +1125,9 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -1070,9 +1137,9 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -1082,9 +1149,9 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1094,9 +1161,9 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -1106,9 +1173,9 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1118,9 +1185,9 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -1130,9 +1197,9 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1142,9 +1209,9 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -1154,9 +1221,9 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -1166,9 +1233,9 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -1178,9 +1245,9 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -1190,9 +1257,9 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -1202,9 +1269,9 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -1214,9 +1281,9 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -1226,9 +1293,9 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-    </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -1238,9 +1305,9 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-    </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -1250,9 +1317,9 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
-    </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -1262,9 +1329,9 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-    </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -1274,9 +1341,9 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-    </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -1286,9 +1353,9 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
-    </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -1298,9 +1365,9 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-    </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -1310,31 +1377,21 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-    </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D79" xr:uid="{36396C9C-E31E-42BE-BB9E-6AB690B20C48}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D64:D79 C2:C62" xr:uid="{36396C9C-E31E-42BE-BB9E-6AB690B20C48}">
       <formula1>"AGROTURISM,ALBERGUE,APART,APARTHOTEL,AP_RURAL,BALNEARIO,BUNGALOW,CAMPING,CASA,CASA_HUESP,CASA_RURAL,CHALET,GLAMPING,HABITACION,HOSTAL,HOTEL,H_RURAL,MOTEL,OFIC_VEHIC,PARADOR,PENSION,REFUGIO,RESIDENCIA,VFT,VILLA,VUT,OTRO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I79" xr:uid="{833F56E2-DFD2-4298-B77A-81B17F17DB34}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I64:I79 H2:H62" xr:uid="{833F56E2-DFD2-4298-B77A-81B17F17DB34}">
       <formula1>"ESP,ARG,USA,MEX,FRA,DEU,ITA,GBR,COL,JPN,CHN,BRA,CAN,MRC,AUS,PRT,BEL,NLD,SWE,CHE,POL,RUS,IND,KOR,PER,GRC,DNK,TUR,EGY,TUN,ARE,SAU,ISR,VEN,CHE,BGR,SVK,HUN,ROU,LTU,LVA,EST,LUX,CZE,CYP,MDA,MLT,CYP,HRV,SVN,BHS,LKA,PAK,IRL,MYS,KWT,PHL,ZAF,THA,NZL,UGA,KEN,TGO,GHA"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{182AB33E-8598-40A6-8BE2-A30B590B9FC2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>